<commit_message>
Update reviews for parisk
</commit_message>
<xml_diff>
--- a/reviews/parisk_20240725_031640.xlsx
+++ b/reviews/parisk_20240725_031640.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,6 +607,51 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>parisk</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>DIS</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WRI</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>53dcf950-aee9-43ba-bb93-9e7c5cd5833d</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>By5SY2gA-_annotated.xlsx</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>For instance, what about averaging WordNet path-based distance metrics and distance in word embedding space (for word similarity), and other ways of applying the affect data to email tone prediction?</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>